<commit_message>
Reworked preparing and processing examples.
</commit_message>
<xml_diff>
--- a/example/info/02 fitting info.xlsx
+++ b/example/info/02 fitting info.xlsx
@@ -579,10 +579,10 @@
         <v>74.37073472538241</v>
       </c>
       <c r="N2" t="n">
-        <v>63702.73562050128</v>
+        <v>63702.73562050127</v>
       </c>
       <c r="O2" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -1924,22 +1924,22 @@
         <v>3.175</v>
       </c>
       <c r="J21" t="n">
-        <v>0.003099591938446999</v>
+        <v>0.003099591938446897</v>
       </c>
       <c r="K21" t="n">
         <v>184.962353082935</v>
       </c>
       <c r="L21" t="n">
-        <v>9.850138957700593e-05</v>
+        <v>9.850138957700202e-05</v>
       </c>
       <c r="M21" t="n">
         <v>5.87788623789952</v>
       </c>
       <c r="N21" t="n">
-        <v>59673.13012680225</v>
+        <v>59673.13012680422</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -2066,22 +2066,22 @@
         <v>3.175</v>
       </c>
       <c r="J23" t="n">
-        <v>0.002986865689476004</v>
+        <v>0.002986865689476005</v>
       </c>
       <c r="K23" t="n">
         <v>176.979439785403</v>
       </c>
       <c r="L23" t="n">
-        <v>0.001295917891209504</v>
+        <v>0.001295917891209503</v>
       </c>
       <c r="M23" t="n">
         <v>76.786453171376</v>
       </c>
       <c r="N23" t="n">
-        <v>59252.56043784517</v>
+        <v>59252.56043784516</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -2137,22 +2137,22 @@
         <v>3.175</v>
       </c>
       <c r="J24" t="n">
-        <v>0.002913928760891336</v>
+        <v>0.002913928760891335</v>
       </c>
       <c r="K24" t="n">
         <v>164.528068453978</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0002542523812495351</v>
+        <v>0.0002542523812495349</v>
       </c>
       <c r="M24" t="n">
         <v>14.3557569931856</v>
       </c>
       <c r="N24" t="n">
-        <v>56462.62553229024</v>
+        <v>56462.62553229026</v>
       </c>
       <c r="O24" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -2208,22 +2208,22 @@
         <v>3.175</v>
       </c>
       <c r="J25" t="n">
-        <v>0.002799291831076499</v>
+        <v>0.0027992918310763</v>
       </c>
       <c r="K25" t="n">
         <v>166.148394269309</v>
       </c>
       <c r="L25" t="n">
-        <v>9.34867799287871e-06</v>
+        <v>9.348677992879577e-06</v>
       </c>
       <c r="M25" t="n">
         <v>0.554878851791746</v>
       </c>
       <c r="N25" t="n">
-        <v>59353.72383286482</v>
+        <v>59353.72383286903</v>
       </c>
       <c r="O25" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>-4.336808689942018e-19</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -2279,22 +2279,22 @@
         <v>3.175</v>
       </c>
       <c r="J26" t="n">
-        <v>0.002342094147758199</v>
+        <v>0.002342094147757995</v>
       </c>
       <c r="K26" t="n">
         <v>143.264709458966</v>
       </c>
       <c r="L26" t="n">
-        <v>6.561829182213455e-05</v>
+        <v>6.561829182212935e-05</v>
       </c>
       <c r="M26" t="n">
         <v>4.01383758295543</v>
       </c>
       <c r="N26" t="n">
-        <v>61169.49209582195</v>
+        <v>61169.49209582728</v>
       </c>
       <c r="O26" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -2350,22 +2350,22 @@
         <v>3.175</v>
       </c>
       <c r="J27" t="n">
-        <v>0.001877897583311999</v>
+        <v>0.001877897583311898</v>
       </c>
       <c r="K27" t="n">
         <v>114.945593796641</v>
       </c>
       <c r="L27" t="n">
-        <v>4.202040312191342e-05</v>
+        <v>4.202040312191104e-05</v>
       </c>
       <c r="M27" t="n">
         <v>2.57205730032622</v>
       </c>
       <c r="N27" t="n">
-        <v>61209.72454414391</v>
+        <v>61209.72454414721</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>2.168404344971009e-19</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -2705,19 +2705,19 @@
         <v>3.175</v>
       </c>
       <c r="J32" t="n">
-        <v>0.0005420269248841921</v>
+        <v>0.0005420269248840922</v>
       </c>
       <c r="K32" t="n">
         <v>46.1272742639521</v>
       </c>
       <c r="L32" t="n">
-        <v>4.254760559953716e-05</v>
+        <v>4.254760559952936e-05</v>
       </c>
       <c r="M32" t="n">
         <v>3.62086269641244</v>
       </c>
       <c r="N32" t="n">
-        <v>85101.44449707461</v>
+        <v>85101.4444970903</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
@@ -2995,16 +2995,16 @@
         <v>144.025333226662</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0007298762958923013</v>
+        <v>0.0007298762958923019</v>
       </c>
       <c r="M36" t="n">
         <v>40.5162310159823</v>
       </c>
       <c r="N36" t="n">
-        <v>55511.09310441386</v>
+        <v>55511.09310441385</v>
       </c>
       <c r="O36" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -3202,22 +3202,22 @@
         <v>3.175</v>
       </c>
       <c r="J39" t="n">
-        <v>0.003535944426428287</v>
+        <v>0.003535944426428288</v>
       </c>
       <c r="K39" t="n">
         <v>176.304083740973</v>
       </c>
       <c r="L39" t="n">
-        <v>0.001604180994517587</v>
+        <v>0.001604180994517588</v>
       </c>
       <c r="M39" t="n">
         <v>79.9853239432246</v>
       </c>
       <c r="N39" t="n">
-        <v>49860.53582269123</v>
+        <v>49860.53582269122</v>
       </c>
       <c r="O39" t="n">
-        <v>-4.336808689942018e-19</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -3699,22 +3699,22 @@
         <v>3.175</v>
       </c>
       <c r="J46" t="n">
-        <v>0.001642667931312868</v>
+        <v>0.001642667931312869</v>
       </c>
       <c r="K46" t="n">
         <v>86.96884979516319</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0008846657864568689</v>
+        <v>0.0008846657864568681</v>
       </c>
       <c r="M46" t="n">
         <v>46.8374431829298</v>
       </c>
       <c r="N46" t="n">
-        <v>52943.65838484175</v>
+        <v>52943.65838484174</v>
       </c>
       <c r="O46" t="n">
-        <v>-4.336808689942018e-19</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
@@ -3776,16 +3776,16 @@
         <v>98.3135045128474</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0002692857965243174</v>
+        <v>0.0002692857965243189</v>
       </c>
       <c r="M47" t="n">
         <v>13.0435931132256</v>
       </c>
       <c r="N47" t="n">
-        <v>48437.73151640275</v>
+        <v>48437.73151640274</v>
       </c>
       <c r="O47" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>-4.336808689942018e-19</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
@@ -4419,16 +4419,16 @@
         <v>126.804257125663</v>
       </c>
       <c r="L56" t="n">
-        <v>0.0009362218356743739</v>
+        <v>0.0009362218356743733</v>
       </c>
       <c r="M56" t="n">
         <v>46.9007946489988</v>
       </c>
       <c r="N56" t="n">
-        <v>50095.81368631023</v>
+        <v>50095.81368631024</v>
       </c>
       <c r="O56" t="n">
-        <v>0</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -4701,22 +4701,22 @@
         <v>3.175</v>
       </c>
       <c r="J60" t="n">
-        <v>0.002183439006668278</v>
+        <v>0.002183439006668277</v>
       </c>
       <c r="K60" t="n">
         <v>114.21692709225</v>
       </c>
       <c r="L60" t="n">
-        <v>0.001216178373921078</v>
+        <v>0.001216178373921077</v>
       </c>
       <c r="M60" t="n">
         <v>63.6189773293808</v>
       </c>
       <c r="N60" t="n">
-        <v>52310.56454676711</v>
+        <v>52310.56454676712</v>
       </c>
       <c r="O60" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -4930,10 +4930,10 @@
         <v>61.8332029123926</v>
       </c>
       <c r="N63" t="n">
-        <v>51251.21984452444</v>
+        <v>51251.21984452443</v>
       </c>
       <c r="O63" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P63" t="inlineStr">
         <is>
@@ -5277,22 +5277,22 @@
         <v>3.175</v>
       </c>
       <c r="J68" t="n">
-        <v>0.004027151846017031</v>
+        <v>0.004027151846017286</v>
       </c>
       <c r="K68" t="n">
         <v>165.156659126179</v>
       </c>
       <c r="L68" t="n">
-        <v>0.002438382967616403</v>
+        <v>0.002438382967616558</v>
       </c>
       <c r="M68" t="n">
         <v>100</v>
       </c>
       <c r="N68" t="n">
-        <v>41010.78515068252</v>
+        <v>41010.78515067993</v>
       </c>
       <c r="O68" t="n">
-        <v>0.0009581021085890004</v>
+        <v>0.0009581021085887454</v>
       </c>
       <c r="P68" t="inlineStr">
         <is>
@@ -5358,16 +5358,16 @@
         <v>188.358407583882</v>
       </c>
       <c r="L69" t="n">
-        <v>0.001009341110338465</v>
+        <v>0.001009341110338467</v>
       </c>
       <c r="M69" t="n">
         <v>44.0232438640259</v>
       </c>
       <c r="N69" t="n">
-        <v>43615.82364287472</v>
+        <v>43615.82364287471</v>
       </c>
       <c r="O69" t="n">
-        <v>8.673617379884035e-19</v>
+        <v>0</v>
       </c>
       <c r="P69" t="inlineStr">
         <is>
@@ -5500,16 +5500,16 @@
         <v>89.5786348354455</v>
       </c>
       <c r="L71" t="n">
-        <v>0.000774351984478844</v>
+        <v>0.0007743519844788433</v>
       </c>
       <c r="M71" t="n">
         <v>28.9731903230109</v>
       </c>
       <c r="N71" t="n">
-        <v>37416.04709970555</v>
+        <v>37416.04709970556</v>
       </c>
       <c r="O71" t="n">
-        <v>0</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P71" t="inlineStr">
         <is>
@@ -6068,16 +6068,16 @@
         <v>60.0918208946391</v>
       </c>
       <c r="L79" t="n">
-        <v>0.0008311687471325137</v>
+        <v>0.000831168747132514</v>
       </c>
       <c r="M79" t="n">
         <v>35.9240131779057</v>
       </c>
       <c r="N79" t="n">
-        <v>43221.08272458698</v>
+        <v>43221.08272458697</v>
       </c>
       <c r="O79" t="n">
-        <v>2.168404344971009e-19</v>
+        <v>0</v>
       </c>
       <c r="P79" t="inlineStr">
         <is>
@@ -6492,22 +6492,22 @@
         <v>3.175</v>
       </c>
       <c r="J85" t="n">
-        <v>0.001133706609370296</v>
+        <v>0.001133706609370197</v>
       </c>
       <c r="K85" t="n">
         <v>56.9308587258361</v>
       </c>
       <c r="L85" t="n">
-        <v>2.996225910133042e-05</v>
+        <v>2.996225910132739e-05</v>
       </c>
       <c r="M85" t="n">
         <v>1.50460191896753</v>
       </c>
       <c r="N85" t="n">
-        <v>50216.57124982067</v>
+        <v>50216.57124982507</v>
       </c>
       <c r="O85" t="n">
-        <v>-4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P85" t="inlineStr">
         <is>
@@ -6634,22 +6634,22 @@
         <v>3.175</v>
       </c>
       <c r="J87" t="n">
-        <v>0.001197085137900892</v>
+        <v>0.001197085137900793</v>
       </c>
       <c r="K87" t="n">
         <v>51.8909929303517</v>
       </c>
       <c r="L87" t="n">
-        <v>8.908567772308797e-05</v>
+        <v>8.908567772308016e-05</v>
       </c>
       <c r="M87" t="n">
         <v>3.86166708328733</v>
       </c>
       <c r="N87" t="n">
-        <v>43347.78812920808</v>
+        <v>43347.78812921167</v>
       </c>
       <c r="O87" t="n">
-        <v>0</v>
+        <v>4.336808689942018e-19</v>
       </c>
       <c r="P87" t="inlineStr">
         <is>
@@ -6853,16 +6853,16 @@
         <v>56.27423602054</v>
       </c>
       <c r="L90" t="n">
-        <v>0.0009467802092584647</v>
+        <v>0.000946780209258465</v>
       </c>
       <c r="M90" t="n">
         <v>39.677883454939</v>
       </c>
       <c r="N90" t="n">
-        <v>41908.23072444176</v>
+        <v>41908.23072444175</v>
       </c>
       <c r="O90" t="n">
-        <v>2.168404344971009e-19</v>
+        <v>0</v>
       </c>
       <c r="P90" t="inlineStr">
         <is>
@@ -7135,19 +7135,19 @@
         <v>3.175</v>
       </c>
       <c r="J94" t="n">
-        <v>0.0009501033114772988</v>
+        <v>0.0009501033114771959</v>
       </c>
       <c r="K94" t="n">
         <v>43.0868710364167</v>
       </c>
       <c r="L94" t="n">
-        <v>3.835712248292586e-05</v>
+        <v>3.835712248292174e-05</v>
       </c>
       <c r="M94" t="n">
         <v>1.73948282232606</v>
       </c>
       <c r="N94" t="n">
-        <v>45349.66936324187</v>
+        <v>45349.66936324678</v>
       </c>
       <c r="O94" t="n">
         <v>0</v>
@@ -7206,22 +7206,22 @@
         <v>3.175</v>
       </c>
       <c r="J95" t="n">
-        <v>0.0013102739596552</v>
+        <v>0.001310273959654997</v>
       </c>
       <c r="K95" t="n">
         <v>59.7216564670194</v>
       </c>
       <c r="L95" t="n">
-        <v>2.03080976708099e-05</v>
+        <v>2.030809767080685e-05</v>
       </c>
       <c r="M95" t="n">
         <v>0.9256333178703851</v>
       </c>
       <c r="N95" t="n">
-        <v>45579.51871586858</v>
+        <v>45579.51871587562</v>
       </c>
       <c r="O95" t="n">
-        <v>4.336808689942018e-19</v>
+        <v>0</v>
       </c>
       <c r="P95" t="inlineStr">
         <is>

</xml_diff>